<commit_message>
Actualizada planilla de resolución de sistemas de ecuaciones lineales
</commit_message>
<xml_diff>
--- a/Linear Equation Systems - Gauss-Seidel Method.xlsx
+++ b/Linear Equation Systems - Gauss-Seidel Method.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramiro Olivencia\WebstormProjects\matematica-superior\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7F41B125-DDAD-4604-BBC1-D0DF639251AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8DC30BAE-F4A9-4076-B9ED-8C7678B6582B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="17055" windowWidth="2400" windowHeight="585"/>
+    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Gauss Seidel 2x2" sheetId="5" r:id="rId1"/>
@@ -965,297 +965,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>11</xdr:col>
-          <xdr:colOff>381000</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>15</xdr:col>
-          <xdr:colOff>457200</xdr:colOff>
-          <xdr:row>16</xdr:row>
-          <xdr:rowOff>104775</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="Object 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1025"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{368E1DE6-DC2D-404B-8F14-C67B2C1567E3}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFE1"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>11</xdr:col>
-          <xdr:colOff>247650</xdr:colOff>
-          <xdr:row>19</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>15</xdr:col>
-          <xdr:colOff>381000</xdr:colOff>
-          <xdr:row>29</xdr:row>
-          <xdr:rowOff>76200</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1026" name="Object 2" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1026"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97DD5888-349A-4DA7-8A22-D63C1F152566}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFE1"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>552450</xdr:colOff>
-          <xdr:row>15</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>10</xdr:col>
-          <xdr:colOff>161925</xdr:colOff>
-          <xdr:row>26</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1028" name="Object 4" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1028"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C600E676-967C-41DB-9C96-BC0DF156959F}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>10</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>0</xdr:row>
-          <xdr:rowOff>104775</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>15</xdr:col>
-          <xdr:colOff>180975</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1029" name="Object 5" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1029"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{352B1DBF-9CF6-4AD6-AD31-D2FB662EFCC1}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFF00" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="13"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>11</xdr:col>
-          <xdr:colOff>57150</xdr:colOff>
-          <xdr:row>31</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>15</xdr:col>
-          <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>40</xdr:row>
-          <xdr:rowOff>104775</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1030" name="Object 6" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1030"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{489F3ACD-76D8-4346-B905-C80EF1AFBA00}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFE1"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -1582,7 +1291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -2470,12 +2179,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A3:E120"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:E11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3385,134 +3094,5 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <oleObjects>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="Equation.3" shapeId="1025" r:id="rId4">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId5">
-            <anchor moveWithCells="1" sizeWithCells="1">
-              <from>
-                <xdr:col>11</xdr:col>
-                <xdr:colOff>381000</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>15</xdr:col>
-                <xdr:colOff>457200</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="Equation.3" shapeId="1025" r:id="rId4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="Equation.3" shapeId="1026" r:id="rId6">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId7">
-            <anchor moveWithCells="1" sizeWithCells="1">
-              <from>
-                <xdr:col>11</xdr:col>
-                <xdr:colOff>247650</xdr:colOff>
-                <xdr:row>19</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>15</xdr:col>
-                <xdr:colOff>381000</xdr:colOff>
-                <xdr:row>29</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="Equation.3" shapeId="1026" r:id="rId6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="Equation.3" shapeId="1028" r:id="rId8">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId9">
-            <anchor moveWithCells="1" sizeWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>552450</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>161925</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="Equation.3" shapeId="1028" r:id="rId8"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="Equation.3" shapeId="1029" r:id="rId10">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId11">
-            <anchor moveWithCells="1" sizeWithCells="1">
-              <from>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>228600</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>15</xdr:col>
-                <xdr:colOff>180975</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="Equation.3" shapeId="1029" r:id="rId10"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="Equation.3" shapeId="1030" r:id="rId12">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId13">
-            <anchor moveWithCells="1" sizeWithCells="1">
-              <from>
-                <xdr:col>11</xdr:col>
-                <xdr:colOff>57150</xdr:colOff>
-                <xdr:row>31</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>15</xdr:col>
-                <xdr:colOff>304800</xdr:colOff>
-                <xdr:row>40</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="Equation.3" shapeId="1030" r:id="rId12"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-  </oleObjects>
 </worksheet>
 </file>
</xml_diff>